<commit_message>
Daily Meeting : Updates
Daily Meeting : Updates
</commit_message>
<xml_diff>
--- a/SmartStore/Documents/Misc/Working.xlsx
+++ b/SmartStore/Documents/Misc/Working.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartSVN\MMO\SmartStore\Documents\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96206969-4E0A-43D9-82A4-683EB82B15F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FDC0CE-5110-4F29-8470-596C3FCC3F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1560" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="18Dec2022" sheetId="8" r:id="rId1"/>
-    <sheet name="02Dec2022" sheetId="2" r:id="rId2"/>
-    <sheet name="01Dec2022" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
-    <sheet name="NoSQL" sheetId="7" r:id="rId8"/>
+    <sheet name="21Dec2022" sheetId="9" r:id="rId1"/>
+    <sheet name="18Dec2022" sheetId="8" r:id="rId2"/>
+    <sheet name="02Dec2022" sheetId="2" r:id="rId3"/>
+    <sheet name="01Dec2022" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId8"/>
+    <sheet name="NoSQL" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="291">
   <si>
     <t>Smart Store</t>
   </si>
@@ -902,12 +903,75 @@
   <si>
     <t xml:space="preserve">Colgate Original 50 g </t>
   </si>
+  <si>
+    <t xml:space="preserve">Credit Days </t>
+  </si>
+  <si>
+    <t>Average Sale per day</t>
+  </si>
+  <si>
+    <t>Sale in a Delivery Cycle</t>
+  </si>
+  <si>
+    <t>Delivery Cycle in days</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Std Delivey Qty</t>
+  </si>
+  <si>
+    <t>Inventroy Before Delivery</t>
+  </si>
+  <si>
+    <t>Delivery No</t>
+  </si>
+  <si>
+    <t>Delivery Quantity</t>
+  </si>
+  <si>
+    <t>Standary Delivery Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory After Delivery </t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Sold Before Next Delivery</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Payment Due by  Date</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>Current Date</t>
+  </si>
+  <si>
+    <t>Remaining Inventory</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Remaining Days for Payment</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -923,8 +987,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,8 +1015,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -978,11 +1062,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1017,11 +1169,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1032,6 +1218,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25707084-C3F6-49A3-872C-D79FB3A32550}" name="Table2" displayName="Table2" ref="A1:F2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F2" xr:uid="{25707084-C3F6-49A3-872C-D79FB3A32550}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{90F4BE1F-D3DA-4925-B3AF-76AB09EA2FF6}" name="Credit Days "/>
+    <tableColumn id="2" xr3:uid="{EE0BF025-53C1-46C5-B34E-39B4E1ABD984}" name="Average Sale per day"/>
+    <tableColumn id="3" xr3:uid="{5CA11825-72F7-4467-8788-62F4E4FDBF8C}" name="Delivery Cycle in days"/>
+    <tableColumn id="4" xr3:uid="{48262135-F278-45CE-AE38-ABDD51538ABC}" name="Sale in a Delivery Cycle">
+      <calculatedColumnFormula>B2*C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{ECC30D0F-4D32-486B-A7B5-2A8D06C72DE8}" name="Buffer" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D2AEDAB7-A023-42A9-B887-CA115FFB47D9}" name="Std Delivey Qty">
+      <calculatedColumnFormula>D2+(D2*E2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1296,10 +1501,266 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895A9895-4E18-4ACC-96BF-12A3E1406598}">
+  <dimension ref="A1:R10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="8" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="12" width="12.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="18" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <f>D2+(D2*E2)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H4" s="13">
+        <v>44931</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G6" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G7" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="H7" s="28">
+        <v>44916</v>
+      </c>
+      <c r="I7" s="29">
+        <v>10</v>
+      </c>
+      <c r="J7" s="29">
+        <v>200</v>
+      </c>
+      <c r="K7" s="29">
+        <f>J7-I7</f>
+        <v>190</v>
+      </c>
+      <c r="L7" s="29">
+        <f>K7+I7</f>
+        <v>200</v>
+      </c>
+      <c r="M7" s="29">
+        <v>60</v>
+      </c>
+      <c r="N7" s="28">
+        <f>'21Dec2022'!$H7+15</f>
+        <v>44931</v>
+      </c>
+      <c r="O7" s="30">
+        <f>_xlfn.DAYS(H4,H7)</f>
+        <v>15</v>
+      </c>
+      <c r="P7" s="30">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="31">
+        <f>_xlfn.DAYS(N7,H4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G8" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="H8" s="33">
+        <f>H7+5</f>
+        <v>44921</v>
+      </c>
+      <c r="I8" s="34">
+        <f>L7-M7</f>
+        <v>140</v>
+      </c>
+      <c r="J8" s="34">
+        <f>J7</f>
+        <v>200</v>
+      </c>
+      <c r="K8" s="29">
+        <f>J8-I8</f>
+        <v>60</v>
+      </c>
+      <c r="L8" s="29">
+        <f>K8+I8</f>
+        <v>200</v>
+      </c>
+      <c r="M8" s="34">
+        <v>40</v>
+      </c>
+      <c r="N8" s="33">
+        <f>'21Dec2022'!$H8+15</f>
+        <v>44936</v>
+      </c>
+      <c r="O8" s="35">
+        <f>_xlfn.DAYS(H4,H8)</f>
+        <v>10</v>
+      </c>
+      <c r="P8" s="35">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="31">
+        <f>_xlfn.DAYS(N8,H4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G9" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="H9" s="33">
+        <f>H8+5</f>
+        <v>44926</v>
+      </c>
+      <c r="I9" s="34">
+        <f>L8-M8</f>
+        <v>160</v>
+      </c>
+      <c r="J9" s="34">
+        <f>J8</f>
+        <v>200</v>
+      </c>
+      <c r="K9" s="29">
+        <f>J9-I9</f>
+        <v>40</v>
+      </c>
+      <c r="L9" s="29">
+        <f>K9+I9</f>
+        <v>200</v>
+      </c>
+      <c r="M9" s="29">
+        <v>50</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G10" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H10" s="33">
+        <f>H9+5</f>
+        <v>44931</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05017269-DD9A-4557-A2A5-45D511A37A72}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -1715,7 +2176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B36C26-1E5B-4948-AB31-78D6977E3E12}">
   <dimension ref="C2:P35"/>
   <sheetViews>
@@ -1973,7 +2434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:V27"/>
   <sheetViews>
@@ -2245,7 +2706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BA28CA-67D8-4BCF-A68C-482BB86AEB00}">
   <dimension ref="A1:O25"/>
   <sheetViews>
@@ -2529,7 +2990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B5A8E8-159B-44AC-AA58-BA25A740A2E1}">
   <dimension ref="A2:E29"/>
   <sheetViews>
@@ -2734,7 +3195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E2B513-F2C8-4386-973A-59B4FC26D85D}">
   <dimension ref="A8:M23"/>
   <sheetViews>
@@ -3062,7 +3523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6379C4-C259-44D3-9F64-238EAA058887}">
   <dimension ref="C1:AG52"/>
   <sheetViews>
@@ -4028,7 +4489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89685D1-B95D-4542-8CB3-CBBA3F8B6904}">
   <dimension ref="A1:W31"/>
   <sheetViews>

</xml_diff>